<commit_message>
Added transmission abroad for other connections
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/Hydro inflows 2017.xlsx
+++ b/dati_casoStudioItalia/Hydro inflows 2017.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0954659\PycharmProjects\DrinDrin---Mix-energetico\dati_casoStudioItalia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE33E087-FDB3-4F9B-B203-E1E7958E268D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E73A9EE-5DF6-4567-A191-C19D8F4D8C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{92FCA223-964B-46AD-B6BA-58318D23218B}"/>
+    <workbookView xWindow="-46188" yWindow="2640" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{92FCA223-964B-46AD-B6BA-58318D23218B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydro_inflows" sheetId="1" r:id="rId1"/>
@@ -199,7 +199,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
   <si>
     <t>NORD</t>
   </si>
@@ -256,6 +256,21 @@
   </si>
   <si>
     <t>PS Closed - GWh</t>
+  </si>
+  <si>
+    <t>PS size</t>
+  </si>
+  <si>
+    <t>PS out</t>
+  </si>
+  <si>
+    <t>PS in</t>
+  </si>
+  <si>
+    <t>PS out ratio</t>
+  </si>
+  <si>
+    <t>PS in ratio</t>
   </si>
 </sst>
 </file>
@@ -390,7 +405,7 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -413,6 +428,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -753,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0F2086-3617-4245-B76A-3A42AFC8BB10}">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2150,8 +2166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3912C844-DC67-4666-8DCD-62AEE8064983}">
   <dimension ref="A1:H366"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A366"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11679,8 +11695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F5EDF29-60C7-486F-84D1-2EA5C70D3E34}">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:G53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12917,10 +12933,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8050974-AF2A-4F6B-8D0D-5A3795C6AE4A}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H14"/>
+      <selection activeCell="J14" sqref="J13:J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13242,6 +13258,123 @@
         <v>0</v>
       </c>
     </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="8">
+        <f>B11*1000</f>
+        <v>194000</v>
+      </c>
+      <c r="C19" s="8">
+        <f t="shared" ref="C19:H19" si="0">C11*1000</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="8">
+        <f t="shared" si="0"/>
+        <v>94990</v>
+      </c>
+      <c r="E19" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="8">
+        <f>B9+B12</f>
+        <v>5205.058</v>
+      </c>
+      <c r="C20" s="8">
+        <f t="shared" ref="C20:H20" si="1">C9+C12</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="8">
+        <f t="shared" si="1"/>
+        <v>1763</v>
+      </c>
+      <c r="E20" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="8">
+        <f t="shared" si="1"/>
+        <v>240</v>
+      </c>
+      <c r="G20" s="8">
+        <f t="shared" si="1"/>
+        <v>580</v>
+      </c>
+      <c r="H20" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <f>B20/B19</f>
+        <v>2.6830195876288661E-2</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ref="D21" si="2">D20/D19</f>
+        <v>1.8559848405095274E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="8">
+        <f>-B10</f>
+        <v>1751</v>
+      </c>
+      <c r="C22" s="8">
+        <f t="shared" ref="C22:H22" si="3">-C10</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="8">
+        <f t="shared" si="3"/>
+        <v>333</v>
+      </c>
+      <c r="E22" s="8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="8">
+        <f t="shared" si="3"/>
+        <v>58</v>
+      </c>
+      <c r="H22" s="8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="decimal" operator="lessThanOrEqual" showInputMessage="1" showErrorMessage="1" errorTitle="Value Error" error="Value for pumping rated power must be negative!" sqref="B13:H13 B10:H10" xr:uid="{EF8C4D86-D4BD-413A-B6C6-1543B6A3D7E9}">

</xml_diff>

<commit_message>
Implemented hydro with Hydro_Reservoir.json and PS in PumpedHydro_Open.json combining open and closed storage
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/Hydro inflows 2017.xlsx
+++ b/dati_casoStudioItalia/Hydro inflows 2017.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0954659\PycharmProjects\DrinDrin---Mix-energetico\dati_casoStudioItalia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E73A9EE-5DF6-4567-A191-C19D8F4D8C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E15379F-8490-40FA-AA7D-3A264002BC17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-46188" yWindow="2640" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{92FCA223-964B-46AD-B6BA-58318D23218B}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="1" activeTab="1" xr2:uid="{92FCA223-964B-46AD-B6BA-58318D23218B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydro_inflows" sheetId="1" r:id="rId1"/>
@@ -405,7 +405,7 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -429,6 +429,12 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -769,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0F2086-3617-4245-B76A-3A42AFC8BB10}">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -802,25 +808,25 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="9">
         <v>182.04785899086809</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="9">
         <v>6.9261845639864106</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="9">
         <v>19.240104889383719</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="9">
         <v>18.378093396825399</v>
       </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
-      <c r="H2">
+      <c r="F2" s="9">
+        <v>0</v>
+      </c>
+      <c r="G2" s="9">
+        <v>0</v>
+      </c>
+      <c r="H2" s="8">
         <v>0</v>
       </c>
     </row>
@@ -828,25 +834,25 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="10">
         <v>178.17086439927621</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="10">
         <v>14.13759867497169</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="10">
         <v>28.636447825252102</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="10">
         <v>24.71747812698413</v>
       </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3">
+      <c r="F3" s="9">
+        <v>0</v>
+      </c>
+      <c r="G3" s="9">
+        <v>0</v>
+      </c>
+      <c r="H3" s="8">
         <v>0</v>
       </c>
     </row>
@@ -854,25 +860,25 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="10">
         <v>229.24466091991749</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="10">
         <v>21.393979422423559</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="10">
         <v>41.540201700606772</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="10">
         <v>37.254718616780053</v>
       </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4">
+      <c r="F4" s="9">
+        <v>0</v>
+      </c>
+      <c r="G4" s="9">
+        <v>0</v>
+      </c>
+      <c r="H4" s="8">
         <v>0</v>
       </c>
     </row>
@@ -880,25 +886,25 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="10">
         <v>231.97528980123161</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="10">
         <v>15.550080079275199</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="10">
         <v>35.895610081881181</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="10">
         <v>31.707260036281181</v>
       </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5">
+      <c r="F5" s="9">
+        <v>0</v>
+      </c>
+      <c r="G5" s="9">
+        <v>0</v>
+      </c>
+      <c r="H5" s="8">
         <v>0</v>
       </c>
     </row>
@@ -906,25 +912,25 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="10">
         <v>209.0177143890362</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="10">
         <v>11.688239535673841</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="10">
         <v>40.530846198306797</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="10">
         <v>59.895378367346943</v>
       </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-      <c r="H6">
+      <c r="F6" s="9">
+        <v>0</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0</v>
+      </c>
+      <c r="H6" s="8">
         <v>0</v>
       </c>
     </row>
@@ -932,25 +938,25 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="10">
         <v>150.6678777429897</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="10">
         <v>10.86649629671574</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="10">
         <v>35.393747868471657</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="10">
         <v>40.697530090702962</v>
       </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0</v>
-      </c>
-      <c r="H7">
+      <c r="F7" s="9">
+        <v>0</v>
+      </c>
+      <c r="G7" s="9">
+        <v>0</v>
+      </c>
+      <c r="H7" s="8">
         <v>0</v>
       </c>
     </row>
@@ -958,25 +964,25 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="10">
         <v>162.8355529178414</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="10">
         <v>20.732705356738389</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="10">
         <v>64.607049721719065</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="10">
         <v>36.063648965986403</v>
       </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8">
+      <c r="F8" s="9">
+        <v>0</v>
+      </c>
+      <c r="G8" s="9">
+        <v>0</v>
+      </c>
+      <c r="H8" s="8">
         <v>0</v>
       </c>
     </row>
@@ -984,25 +990,25 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="10">
         <v>140.71550090112069</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="10">
         <v>29.77805287655719</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="10">
         <v>63.064421126937248</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="10">
         <v>24.670566839002259</v>
       </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-      <c r="H9">
+      <c r="F9" s="9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1010,25 +1016,25 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="10">
         <v>141.50229227370281</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="10">
         <v>22.10639201585504</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="10">
         <v>49.232132796661979</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="10">
         <v>20.815095052154199</v>
       </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-      <c r="H10">
+      <c r="F10" s="9">
+        <v>0</v>
+      </c>
+      <c r="G10" s="9">
+        <v>0</v>
+      </c>
+      <c r="H10" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1036,25 +1042,25 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="10">
         <v>143.58230521230479</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="10">
         <v>30.43932694224236</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="10">
         <v>65.914738420785838</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="10">
         <v>18.291426780045349</v>
       </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
-      <c r="H11">
+      <c r="F11" s="9">
+        <v>0</v>
+      </c>
+      <c r="G11" s="9">
+        <v>0</v>
+      </c>
+      <c r="H11" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1062,25 +1068,25 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="10">
         <v>158.85887435144269</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="10">
         <v>28.65036016987543</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="10">
         <v>68.858788330691894</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="10">
         <v>23.832524507936508</v>
       </c>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0</v>
-      </c>
-      <c r="H12">
+      <c r="F12" s="9">
+        <v>0</v>
+      </c>
+      <c r="G12" s="9">
+        <v>0</v>
+      </c>
+      <c r="H12" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1088,25 +1094,25 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="10">
         <v>183.77007766275301</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="10">
         <v>21.38868922989807</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="10">
         <v>51.011065038600528</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="10">
         <v>25.221575696145131</v>
       </c>
-      <c r="F13" s="1">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0</v>
-      </c>
-      <c r="H13">
+      <c r="F13" s="9">
+        <v>0</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0</v>
+      </c>
+      <c r="H13" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1114,25 +1120,25 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="10">
         <v>189.0292973692996</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="10">
         <v>18.709206715741789</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="10">
         <v>47.365774263588193</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="10">
         <v>24.281759723356011</v>
       </c>
-      <c r="F14" s="1">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0</v>
-      </c>
-      <c r="H14">
+      <c r="F14" s="9">
+        <v>0</v>
+      </c>
+      <c r="G14" s="9">
+        <v>0</v>
+      </c>
+      <c r="H14" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1140,25 +1146,25 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="10">
         <v>198.6238799444514</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="10">
         <v>15.411653374858441</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="10">
         <v>40.35760853502719</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="10">
         <v>18.22225250793651</v>
       </c>
-      <c r="F15" s="1">
-        <v>0</v>
-      </c>
-      <c r="G15" s="1">
-        <v>0</v>
-      </c>
-      <c r="H15">
+      <c r="F15" s="9">
+        <v>0</v>
+      </c>
+      <c r="G15" s="9">
+        <v>0</v>
+      </c>
+      <c r="H15" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1166,25 +1172,25 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="10">
         <v>206.001384115642</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="10">
         <v>12.37949135900339</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="10">
         <v>33.554919738942651</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="10">
         <v>16.74176406349207</v>
       </c>
-      <c r="F16" s="1">
-        <v>0</v>
-      </c>
-      <c r="G16" s="1">
-        <v>0</v>
-      </c>
-      <c r="H16">
+      <c r="F16" s="9">
+        <v>0</v>
+      </c>
+      <c r="G16" s="9">
+        <v>0</v>
+      </c>
+      <c r="H16" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1192,25 +1198,25 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="10">
         <v>188.98034541738559</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="10">
         <v>10.1003000792752</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="10">
         <v>25.19254335946539</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="10">
         <v>15.02274364625851</v>
       </c>
-      <c r="F17" s="1">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1">
-        <v>0</v>
-      </c>
-      <c r="H17">
+      <c r="F17" s="9">
+        <v>0</v>
+      </c>
+      <c r="G17" s="9">
+        <v>0</v>
+      </c>
+      <c r="H17" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1218,25 +1224,25 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="10">
         <v>188.44543408828849</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="10">
         <v>9.4385851642129115</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="10">
         <v>25.42597183236558</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="10">
         <v>13.6575456553288</v>
       </c>
-      <c r="F18" s="1">
-        <v>0</v>
-      </c>
-      <c r="G18" s="1">
-        <v>0</v>
-      </c>
-      <c r="H18">
+      <c r="F18" s="9">
+        <v>0</v>
+      </c>
+      <c r="G18" s="9">
+        <v>0</v>
+      </c>
+      <c r="H18" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1244,25 +1250,25 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="10">
         <v>218.74313218112189</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="10">
         <v>13.48999093997735</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="10">
         <v>29.370116440396181</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="10">
         <v>14.58225460317461</v>
       </c>
-      <c r="F19" s="1">
-        <v>0</v>
-      </c>
-      <c r="G19" s="1">
-        <v>0</v>
-      </c>
-      <c r="H19">
+      <c r="F19" s="9">
+        <v>0</v>
+      </c>
+      <c r="G19" s="9">
+        <v>0</v>
+      </c>
+      <c r="H19" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1270,25 +1276,25 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="10">
         <v>203.28232569568931</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="10">
         <v>15.116284292185741</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="10">
         <v>31.835616650547369</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="10">
         <v>15.5705720770975</v>
       </c>
-      <c r="F20" s="1">
-        <v>0</v>
-      </c>
-      <c r="G20" s="1">
-        <v>0</v>
-      </c>
-      <c r="H20">
+      <c r="F20" s="9">
+        <v>0</v>
+      </c>
+      <c r="G20" s="9">
+        <v>0</v>
+      </c>
+      <c r="H20" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1296,25 +1302,25 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="10">
         <v>199.63318018937011</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="10">
         <v>16.159333918459801</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="10">
         <v>32.669819599952781</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="10">
         <v>15.024333859410429</v>
       </c>
-      <c r="F21" s="1">
-        <v>0</v>
-      </c>
-      <c r="G21" s="1">
-        <v>0</v>
-      </c>
-      <c r="H21">
+      <c r="F21" s="9">
+        <v>0</v>
+      </c>
+      <c r="G21" s="9">
+        <v>0</v>
+      </c>
+      <c r="H21" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1322,25 +1328,25 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="10">
         <v>286.66263040861838</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="10">
         <v>20.493324144960361</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="10">
         <v>37.048764475401548</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="10">
         <v>16.56843082993198</v>
       </c>
-      <c r="F22" s="1">
-        <v>0</v>
-      </c>
-      <c r="G22" s="1">
-        <v>0</v>
-      </c>
-      <c r="H22">
+      <c r="F22" s="9">
+        <v>0</v>
+      </c>
+      <c r="G22" s="9">
+        <v>0</v>
+      </c>
+      <c r="H22" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1348,25 +1354,25 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="10">
         <v>288.44626152926821</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="10">
         <v>15.4204703624009</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="10">
         <v>31.919407533319909</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="10">
         <v>17.908185410430839</v>
       </c>
-      <c r="F23" s="1">
-        <v>0</v>
-      </c>
-      <c r="G23" s="1">
-        <v>0</v>
-      </c>
-      <c r="H23">
+      <c r="F23" s="9">
+        <v>0</v>
+      </c>
+      <c r="G23" s="9">
+        <v>0</v>
+      </c>
+      <c r="H23" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1374,25 +1380,25 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="10">
         <v>286.42232082649502</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="10">
         <v>15.26881817667044</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="10">
         <v>31.829323367826198</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="10">
         <v>20.361089197278911</v>
       </c>
-      <c r="F24" s="1">
-        <v>0</v>
-      </c>
-      <c r="G24" s="1">
-        <v>0</v>
-      </c>
-      <c r="H24">
+      <c r="F24" s="9">
+        <v>0</v>
+      </c>
+      <c r="G24" s="9">
+        <v>0</v>
+      </c>
+      <c r="H24" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1400,25 +1406,25 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="10">
         <v>314.62665544838609</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="10">
         <v>18.330517100792751</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="10">
         <v>34.250348199901843</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="10">
         <v>19.808490126984129</v>
       </c>
-      <c r="F25" s="1">
-        <v>0</v>
-      </c>
-      <c r="G25" s="1">
-        <v>0</v>
-      </c>
-      <c r="H25">
+      <c r="F25" s="9">
+        <v>0</v>
+      </c>
+      <c r="G25" s="9">
+        <v>0</v>
+      </c>
+      <c r="H25" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1426,25 +1432,25 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="10">
         <v>340.93254437150182</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="10">
         <v>20.109785186862968</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="10">
         <v>35.488843604896559</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="10">
         <v>19.15968316099773</v>
       </c>
-      <c r="F26" s="1">
-        <v>0</v>
-      </c>
-      <c r="G26" s="1">
-        <v>0</v>
-      </c>
-      <c r="H26">
+      <c r="F26" s="9">
+        <v>0</v>
+      </c>
+      <c r="G26" s="9">
+        <v>0</v>
+      </c>
+      <c r="H26" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1452,25 +1458,25 @@
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="10">
         <v>345.24476631738412</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="10">
         <v>14.58946928652321</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="10">
         <v>25.344744583531028</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="10">
         <v>19.145371242630389</v>
       </c>
-      <c r="F27" s="1">
-        <v>0</v>
-      </c>
-      <c r="G27" s="1">
-        <v>0</v>
-      </c>
-      <c r="H27">
+      <c r="F27" s="9">
+        <v>0</v>
+      </c>
+      <c r="G27" s="9">
+        <v>0</v>
+      </c>
+      <c r="H27" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1478,25 +1484,25 @@
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="10">
         <v>350.65618209260901</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="10">
         <v>12.33672896942242</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="10">
         <v>24.452895736573769</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="10">
         <v>21.079070435374149</v>
       </c>
-      <c r="F28" s="1">
-        <v>0</v>
-      </c>
-      <c r="G28" s="1">
-        <v>0</v>
-      </c>
-      <c r="H28">
+      <c r="F28" s="9">
+        <v>0</v>
+      </c>
+      <c r="G28" s="9">
+        <v>0</v>
+      </c>
+      <c r="H28" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1504,25 +1510,25 @@
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="10">
         <v>364.62350902691861</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="10">
         <v>13.30527505096263</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="10">
         <v>23.665851703288311</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="10">
         <v>21.519559478458049</v>
       </c>
-      <c r="F29" s="1">
-        <v>0</v>
-      </c>
-      <c r="G29" s="1">
-        <v>0</v>
-      </c>
-      <c r="H29">
+      <c r="F29" s="9">
+        <v>0</v>
+      </c>
+      <c r="G29" s="9">
+        <v>0</v>
+      </c>
+      <c r="H29" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1530,25 +1536,25 @@
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="10">
         <v>334.7601482528861</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="10">
         <v>13.85633677236693</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="10">
         <v>23.75566408614084</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="10">
         <v>18.80824605442178</v>
       </c>
-      <c r="F30" s="1">
-        <v>0</v>
-      </c>
-      <c r="G30" s="1">
-        <v>0</v>
-      </c>
-      <c r="H30">
+      <c r="F30" s="9">
+        <v>0</v>
+      </c>
+      <c r="G30" s="9">
+        <v>0</v>
+      </c>
+      <c r="H30" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1556,25 +1562,25 @@
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="10">
         <v>345.07298946794032</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="10">
         <v>9.8137479841449586</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="10">
         <v>20.279848089048091</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31" s="10">
         <v>18.324821256235829</v>
       </c>
-      <c r="F31" s="1">
-        <v>0</v>
-      </c>
-      <c r="G31" s="1">
-        <v>0</v>
-      </c>
-      <c r="H31">
+      <c r="F31" s="9">
+        <v>0</v>
+      </c>
+      <c r="G31" s="9">
+        <v>0</v>
+      </c>
+      <c r="H31" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1582,25 +1588,25 @@
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="10">
         <v>353.64225115936529</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="10">
         <v>9.142775232163082</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="10">
         <v>20.479953107199901</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32" s="10">
         <v>18.785187963718819</v>
       </c>
-      <c r="F32" s="1">
-        <v>0</v>
-      </c>
-      <c r="G32" s="1">
-        <v>0</v>
-      </c>
-      <c r="H32">
+      <c r="F32" s="9">
+        <v>0</v>
+      </c>
+      <c r="G32" s="9">
+        <v>0</v>
+      </c>
+      <c r="H32" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1608,25 +1614,25 @@
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="10">
         <v>350.29037750648757</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="10">
         <v>9.9676044167610414</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="10">
         <v>20.324486494636741</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33" s="10">
         <v>19.08255782312925</v>
       </c>
-      <c r="F33" s="1">
-        <v>0</v>
-      </c>
-      <c r="G33" s="1">
-        <v>0</v>
-      </c>
-      <c r="H33">
+      <c r="F33" s="9">
+        <v>0</v>
+      </c>
+      <c r="G33" s="9">
+        <v>0</v>
+      </c>
+      <c r="H33" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1634,25 +1640,25 @@
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="10">
         <v>310.26103137314311</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="10">
         <v>8.1927448244620606</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="10">
         <v>15.178944181056229</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="10">
         <v>19.023719936507931</v>
       </c>
-      <c r="F34" s="1">
-        <v>0</v>
-      </c>
-      <c r="G34" s="1">
-        <v>0</v>
-      </c>
-      <c r="H34">
+      <c r="F34" s="9">
+        <v>0</v>
+      </c>
+      <c r="G34" s="9">
+        <v>0</v>
+      </c>
+      <c r="H34" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1660,25 +1666,25 @@
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="10">
         <v>297.57268543702389</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="10">
         <v>8.1257357191392963</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="10">
         <v>15.684887761961029</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="10">
         <v>19.284514893424031</v>
       </c>
-      <c r="F35" s="1">
-        <v>0</v>
-      </c>
-      <c r="G35" s="1">
-        <v>0</v>
-      </c>
-      <c r="H35">
+      <c r="F35" s="9">
+        <v>0</v>
+      </c>
+      <c r="G35" s="9">
+        <v>0</v>
+      </c>
+      <c r="H35" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1686,25 +1692,25 @@
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="10">
         <v>302.99923181556761</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="10">
         <v>7.7593898867497169</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="10">
         <v>15.17250217517152</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36" s="10">
         <v>16.950081986394562</v>
       </c>
-      <c r="F36" s="1">
-        <v>0</v>
-      </c>
-      <c r="G36" s="1">
-        <v>0</v>
-      </c>
-      <c r="H36">
+      <c r="F36" s="9">
+        <v>0</v>
+      </c>
+      <c r="G36" s="9">
+        <v>0</v>
+      </c>
+      <c r="H36" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1712,25 +1718,25 @@
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37" s="10">
         <v>321.66060592068902</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="10">
         <v>8.8769430577576429</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="10">
         <v>15.76584659388371</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37" s="10">
         <v>15.69778912925171</v>
       </c>
-      <c r="F37" s="1">
-        <v>0</v>
-      </c>
-      <c r="G37" s="1">
-        <v>0</v>
-      </c>
-      <c r="H37">
+      <c r="F37" s="9">
+        <v>0</v>
+      </c>
+      <c r="G37" s="9">
+        <v>0</v>
+      </c>
+      <c r="H37" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1738,25 +1744,25 @@
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38" s="10">
         <v>305.20918993561418</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="10">
         <v>8.3796649603624012</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38" s="10">
         <v>13.64659957215777</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38" s="10">
         <v>15.96812536507937</v>
       </c>
-      <c r="F38" s="1">
-        <v>0</v>
-      </c>
-      <c r="G38" s="1">
-        <v>0</v>
-      </c>
-      <c r="H38">
+      <c r="F38" s="9">
+        <v>0</v>
+      </c>
+      <c r="G38" s="9">
+        <v>0</v>
+      </c>
+      <c r="H38" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1764,25 +1770,25 @@
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39" s="10">
         <v>339.49869719816508</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="10">
         <v>8.665776206115515</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39" s="10">
         <v>18.72496802924762</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39" s="10">
         <v>16.664638725623579</v>
       </c>
-      <c r="F39" s="1">
-        <v>0</v>
-      </c>
-      <c r="G39" s="1">
-        <v>0</v>
-      </c>
-      <c r="H39">
+      <c r="F39" s="9">
+        <v>0</v>
+      </c>
+      <c r="G39" s="9">
+        <v>0</v>
+      </c>
+      <c r="H39" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1790,25 +1796,25 @@
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40" s="10">
         <v>304.74904158762217</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="10">
         <v>8.249614394110985</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40" s="10">
         <v>19.76977623079587</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E40" s="10">
         <v>17.498705523809519</v>
       </c>
-      <c r="F40" s="1">
-        <v>0</v>
-      </c>
-      <c r="G40" s="1">
-        <v>0</v>
-      </c>
-      <c r="H40">
+      <c r="F40" s="9">
+        <v>0</v>
+      </c>
+      <c r="G40" s="9">
+        <v>0</v>
+      </c>
+      <c r="H40" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1816,25 +1822,25 @@
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41" s="10">
         <v>253.97963720433719</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="10">
         <v>8.1314667610419029</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41" s="10">
         <v>20.465970184813269</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41" s="10">
         <v>13.49534391383219</v>
       </c>
-      <c r="F41" s="1">
-        <v>0</v>
-      </c>
-      <c r="G41" s="1">
-        <v>0</v>
-      </c>
-      <c r="H41">
+      <c r="F41" s="9">
+        <v>0</v>
+      </c>
+      <c r="G41" s="9">
+        <v>0</v>
+      </c>
+      <c r="H41" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1842,25 +1848,25 @@
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="10">
         <v>231.75545103536311</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="10">
         <v>8.3130967044167612</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42" s="10">
         <v>18.67974735248967</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E42" s="10">
         <v>10.68941280725624</v>
       </c>
-      <c r="F42" s="1">
-        <v>0</v>
-      </c>
-      <c r="G42" s="1">
-        <v>0</v>
-      </c>
-      <c r="H42">
+      <c r="F42" s="9">
+        <v>0</v>
+      </c>
+      <c r="G42" s="9">
+        <v>0</v>
+      </c>
+      <c r="H42" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1868,25 +1874,25 @@
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" s="10">
         <v>205.62489910364849</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="10">
         <v>10.22990979614949</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="10">
         <v>20.649497092928261</v>
       </c>
-      <c r="E43" s="2">
+      <c r="E43" s="10">
         <v>11.9743050340136</v>
       </c>
-      <c r="F43" s="1">
-        <v>0</v>
-      </c>
-      <c r="G43" s="1">
-        <v>0</v>
-      </c>
-      <c r="H43">
+      <c r="F43" s="9">
+        <v>0</v>
+      </c>
+      <c r="G43" s="9">
+        <v>0</v>
+      </c>
+      <c r="H43" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1894,25 +1900,25 @@
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="10">
         <v>186.73656594874379</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="10">
         <v>9.3808338958097384</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44" s="10">
         <v>18.957035275003101</v>
       </c>
-      <c r="E44" s="2">
+      <c r="E44" s="10">
         <v>12.85210269387755</v>
       </c>
-      <c r="F44" s="1">
-        <v>0</v>
-      </c>
-      <c r="G44" s="1">
-        <v>0</v>
-      </c>
-      <c r="H44">
+      <c r="F44" s="9">
+        <v>0</v>
+      </c>
+      <c r="G44" s="9">
+        <v>0</v>
+      </c>
+      <c r="H44" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1920,25 +1926,25 @@
       <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="10">
         <v>160.25712010520559</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="10">
         <v>10.566718720271799</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D45" s="10">
         <v>20.772655859560039</v>
       </c>
-      <c r="E45" s="2">
+      <c r="E45" s="10">
         <v>10.941461591836729</v>
       </c>
-      <c r="F45" s="1">
-        <v>0</v>
-      </c>
-      <c r="G45" s="1">
-        <v>0</v>
-      </c>
-      <c r="H45">
+      <c r="F45" s="9">
+        <v>0</v>
+      </c>
+      <c r="G45" s="9">
+        <v>0</v>
+      </c>
+      <c r="H45" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1946,25 +1952,25 @@
       <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46" s="10">
         <v>156.62933545063049</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="10">
         <v>11.00624554926387</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D46" s="10">
         <v>20.43601266972534</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E46" s="10">
         <v>12.03870866666667</v>
       </c>
-      <c r="F46" s="1">
-        <v>0</v>
-      </c>
-      <c r="G46" s="1">
-        <v>0</v>
-      </c>
-      <c r="H46">
+      <c r="F46" s="9">
+        <v>0</v>
+      </c>
+      <c r="G46" s="9">
+        <v>0</v>
+      </c>
+      <c r="H46" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1972,25 +1978,25 @@
       <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" s="10">
         <v>220.6059764603234</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="10">
         <v>15.212830305775761</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D47" s="10">
         <v>30.001676401397699</v>
       </c>
-      <c r="E47" s="2">
+      <c r="E47" s="10">
         <v>10.095468195011341</v>
       </c>
-      <c r="F47" s="1">
-        <v>0</v>
-      </c>
-      <c r="G47" s="1">
-        <v>0</v>
-      </c>
-      <c r="H47">
+      <c r="F47" s="9">
+        <v>0</v>
+      </c>
+      <c r="G47" s="9">
+        <v>0</v>
+      </c>
+      <c r="H47" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1998,25 +2004,25 @@
       <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48" s="10">
         <v>175.25065795873141</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="10">
         <v>17.032215685164221</v>
       </c>
-      <c r="D48" s="2">
+      <c r="D48" s="10">
         <v>48.337937405306739</v>
       </c>
-      <c r="E48" s="2">
+      <c r="E48" s="10">
         <v>11.967944181405899</v>
       </c>
-      <c r="F48" s="1">
-        <v>0</v>
-      </c>
-      <c r="G48" s="1">
-        <v>0</v>
-      </c>
-      <c r="H48">
+      <c r="F48" s="9">
+        <v>0</v>
+      </c>
+      <c r="G48" s="9">
+        <v>0</v>
+      </c>
+      <c r="H48" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2024,25 +2030,25 @@
       <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49" s="10">
         <v>149.41114763203299</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="10">
         <v>20.626901506228769</v>
       </c>
-      <c r="D49" s="2">
+      <c r="D49" s="10">
         <v>35.532006769260377</v>
       </c>
-      <c r="E49" s="2">
+      <c r="E49" s="10">
         <v>9.1683739274376403</v>
       </c>
-      <c r="F49" s="1">
-        <v>0</v>
-      </c>
-      <c r="G49" s="1">
-        <v>0</v>
-      </c>
-      <c r="H49">
+      <c r="F49" s="9">
+        <v>0</v>
+      </c>
+      <c r="G49" s="9">
+        <v>0</v>
+      </c>
+      <c r="H49" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2050,25 +2056,25 @@
       <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50" s="10">
         <v>169.11920347262549</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="10">
         <v>16.390338992072479</v>
       </c>
-      <c r="D50" s="2">
+      <c r="D50" s="10">
         <v>36.472417831098568</v>
       </c>
-      <c r="E50" s="2">
+      <c r="E50" s="10">
         <v>11.34855615873016</v>
       </c>
-      <c r="F50" s="1">
-        <v>0</v>
-      </c>
-      <c r="G50" s="1">
-        <v>0</v>
-      </c>
-      <c r="H50">
+      <c r="F50" s="9">
+        <v>0</v>
+      </c>
+      <c r="G50" s="9">
+        <v>0</v>
+      </c>
+      <c r="H50" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2076,25 +2082,25 @@
       <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51" s="10">
         <v>149.46810990335109</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="10">
         <v>12.51527296715741</v>
       </c>
-      <c r="D51" s="2">
+      <c r="D51" s="10">
         <v>28.883325121370259</v>
       </c>
-      <c r="E51" s="2">
+      <c r="E51" s="10">
         <v>13.355405156462581</v>
       </c>
-      <c r="F51" s="1">
-        <v>0</v>
-      </c>
-      <c r="G51" s="1">
-        <v>0</v>
-      </c>
-      <c r="H51">
+      <c r="F51" s="9">
+        <v>0</v>
+      </c>
+      <c r="G51" s="9">
+        <v>0</v>
+      </c>
+      <c r="H51" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2102,25 +2108,25 @@
       <c r="A52">
         <v>51</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B52" s="10">
         <v>204.1429900138871</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="10">
         <v>11.990662208380529</v>
       </c>
-      <c r="D52" s="2">
+      <c r="D52" s="10">
         <v>46.360274204204067</v>
       </c>
-      <c r="E52" s="2">
+      <c r="E52" s="10">
         <v>14.33497645804988</v>
       </c>
-      <c r="F52" s="1">
-        <v>0</v>
-      </c>
-      <c r="G52" s="1">
-        <v>0</v>
-      </c>
-      <c r="H52">
+      <c r="F52" s="9">
+        <v>0</v>
+      </c>
+      <c r="G52" s="9">
+        <v>0</v>
+      </c>
+      <c r="H52" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2128,25 +2134,25 @@
       <c r="A53">
         <v>52</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53" s="10">
         <v>177.12596273478371</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="10">
         <v>11.244745062287659</v>
       </c>
-      <c r="D53" s="2">
+      <c r="D53" s="10">
         <v>39.840758518676203</v>
       </c>
-      <c r="E53" s="2">
+      <c r="E53" s="10">
         <v>16.70518916099773</v>
       </c>
-      <c r="F53" s="1">
-        <v>0</v>
-      </c>
-      <c r="G53" s="1">
-        <v>0</v>
-      </c>
-      <c r="H53">
+      <c r="F53" s="9">
+        <v>0</v>
+      </c>
+      <c r="G53" s="9">
+        <v>0</v>
+      </c>
+      <c r="H53" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2166,7 +2172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3912C844-DC67-4666-8DCD-62AEE8064983}">
   <dimension ref="A1:H366"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C24"/>
     </sheetView>
   </sheetViews>
@@ -11695,8 +11701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F5EDF29-60C7-486F-84D1-2EA5C70D3E34}">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D14"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11735,7 +11741,8 @@
         <v>0</v>
       </c>
       <c r="D2" s="1">
-        <v>4.8748487562189062</v>
+        <f>4.87484875621891</f>
+        <v>4.8748487562189098</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -12933,10 +12940,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8050974-AF2A-4F6B-8D0D-5A3795C6AE4A}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J13:J14"/>
+      <selection sqref="A1:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12944,12 +12951,12 @@
     <col min="1" max="1" width="26.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -12972,7 +12979,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -12998,7 +13005,7 @@
         <v>50.03</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -13024,7 +13031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -13050,7 +13057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -13075,8 +13082,12 @@
       <c r="H7" s="4">
         <v>178.27</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7">
+        <f>SUM(B8:H8)*1000/SUM(B7:H7)</f>
+        <v>631.67103089668376</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -13102,7 +13113,7 @@
         <v>153.80000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -13128,7 +13139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
@@ -13154,7 +13165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -13180,7 +13191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
@@ -13206,7 +13217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
@@ -13232,7 +13243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>18</v>
       </c>

</xml_diff>